<commit_message>
database update and test enumeration
</commit_message>
<xml_diff>
--- a/Requisitos/Levantamento Requisitos.xlsx
+++ b/Requisitos/Levantamento Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IPCA\2o Ano\Projeto final\Crypto-Challenge---Documentacao\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF2F5EF-45EB-4313-9144-BFB9FD4F70F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E67B1E5-34E1-4107-BCD7-512C3F687DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A2C320C8-F907-4008-89FE-95236A5C8DBA}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Logica de negócio" sheetId="2" r:id="rId2"/>
     <sheet name="EndPoints" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EndPoints!$A$2:$O$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
   <si>
     <t>Utilizador</t>
   </si>
@@ -503,9 +506,6 @@
     <t>/Users</t>
   </si>
   <si>
-    <t>/CrypoCoin/{id}&lt;showCoinHistory&gt;</t>
-  </si>
-  <si>
     <t>RESTFull URL</t>
   </si>
   <si>
@@ -590,12 +590,6 @@
     <t>start timer</t>
   </si>
   <si>
-    <t>pause timer</t>
-  </si>
-  <si>
-    <t>timer/:id/pause</t>
-  </si>
-  <si>
     <t>AddNewGameTransaction</t>
   </si>
   <si>
@@ -611,9 +605,6 @@
     <t>update gameuser crypto amount</t>
   </si>
   <si>
-    <t>GetSpecificCoinValueHistoric</t>
-  </si>
-  <si>
     <t>GetUserTransactionHistory</t>
   </si>
   <si>
@@ -647,16 +638,55 @@
     <t>GetSepcificCrypto</t>
   </si>
   <si>
-    <t xml:space="preserve">/gameTransaction/:gameId/:userId </t>
-  </si>
-  <si>
-    <t>/gameTransaction/&lt;gameId,userId&gt;</t>
-  </si>
-  <si>
     <t>/GAME/:id</t>
   </si>
   <si>
     <t>GetSpecificGame</t>
+  </si>
+  <si>
+    <t>/Cryptos/:id/currentValue</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>GetSepcificCryptoValue</t>
+  </si>
+  <si>
+    <t>/Cryptos/:id/historicValue</t>
+  </si>
+  <si>
+    <t>GetSepcificCryptoHistoricValue</t>
+  </si>
+  <si>
+    <t>CalculateLeaderBoardForSpecificGame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Transactions/:game/:userId </t>
+  </si>
+  <si>
+    <t>/Transactions/&lt;gameid, userId&gt;</t>
+  </si>
+  <si>
+    <t>GAME</t>
+  </si>
+  <si>
+    <t>TIMER</t>
+  </si>
+  <si>
+    <t>CRYPTO</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>WALLET</t>
+  </si>
+  <si>
+    <t>TRANSACTION</t>
+  </si>
+  <si>
+    <t>/LeaderBoard/:gameId</t>
   </si>
 </sst>
 </file>
@@ -700,18 +730,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -727,7 +751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -736,7 +760,6 @@
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1056,7 +1079,7 @@
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,7 +1124,7 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1225,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FBDC7D-2FAC-4B57-9AB8-B3EA674FEE5E}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1245,16 +1268,16 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1262,10 +1285,13 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
         <v>0</v>
@@ -1273,102 +1299,121 @@
     </row>
     <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
       </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
         <v>50</v>
       </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="O8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
@@ -1377,245 +1422,232 @@
     </row>
     <row r="12" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
       </c>
       <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>75</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>53</v>
-      </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
       </c>
       <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
         <v>74</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="O17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" t="s">
-        <v>73</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
       </c>
       <c r="D19" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="O20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="D21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="O23" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
       <c r="G24" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="G27" s="5"/>
-      <c r="O27" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="G28" s="5"/>
-      <c r="O28" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="5"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
         <v>56</v>
       </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" t="s">
-        <v>58</v>
-      </c>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:O2" xr:uid="{76FBDC7D-2FAC-4B57-9AB8-B3EA674FEE5E}"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{3C08D489-1958-466E-85BF-218AF3652A88}"/>
   </hyperlinks>

</xml_diff>